<commit_message>
feat: fix cohort data model and provide one tree view for 'Variables'
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CohortsLocal.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CohortsLocal.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6645F0A-3FF1-F74F-86ED-C0439825358D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17AE523-4779-9446-95C8-74E3C116414B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
-    <sheet name="Tables" sheetId="13" r:id="rId2"/>
-    <sheet name="Variables" sheetId="3" r:id="rId3"/>
-    <sheet name="VariableHarmonisations" sheetId="4" r:id="rId4"/>
-    <sheet name="CollectionEvents" sheetId="10" r:id="rId5"/>
+    <sheet name="Variables" sheetId="3" r:id="rId2"/>
+    <sheet name="VariableHarmonisations" sheetId="4" r:id="rId3"/>
+    <sheet name="Tables" sheetId="13" r:id="rId4"/>
+    <sheet name="TableHarmonisations" sheetId="14" r:id="rId5"/>
+    <sheet name="CollectionEvents" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$M$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$M$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="146">
   <si>
     <t>name</t>
   </si>
@@ -322,9 +323,6 @@
     <t>AgeCategories</t>
   </si>
   <si>
-    <t>CohortsCentral</t>
-  </si>
-  <si>
     <t>Formats</t>
   </si>
   <si>
@@ -467,13 +465,37 @@
   </si>
   <si>
     <t>Continuous</t>
+  </si>
+  <si>
+    <t>CohortsShared</t>
+  </si>
+  <si>
+    <t>CohortsHarmonised</t>
+  </si>
+  <si>
+    <t>localtable1</t>
+  </si>
+  <si>
+    <t>my table mapping</t>
+  </si>
+  <si>
+    <t>Asthma medication</t>
+  </si>
+  <si>
+    <t>asthma</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>Some asthma question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -502,16 +524,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,12 +560,6 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -591,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -599,8 +607,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -609,12 +615,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,8 +944,8 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,885 +1003,856 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="15">
-        <v>1</v>
-      </c>
-      <c r="G2" s="15" t="s">
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="15">
-        <v>1</v>
-      </c>
-      <c r="L3" s="15" t="s">
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="K8" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="C9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="C10" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="G12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="C13" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="15" t="s">
+      <c r="H13" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="K7" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="K13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="K8" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="K9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="K10" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L10" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="K12" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="15" t="s">
+      <c r="K14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="K15" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="K16" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="16">
-        <v>1</v>
-      </c>
-      <c r="L17" s="16" t="s">
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="L17" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="15" t="s">
+      <c r="F18" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="K18" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L18" s="15" t="s">
+      <c r="K18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K19" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L19" s="15" t="s">
+      <c r="K19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="L20" s="14" t="s">
+      <c r="K20" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K23" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K24" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K30" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="K32" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="16">
+        <v>1</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="L33" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L35" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+    </row>
+    <row r="39" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C39" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="17">
+        <v>1</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="H39" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="21">
-        <v>1</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="I22" s="21" t="s">
+      <c r="F40" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K41" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="L22" s="21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="K42" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="21" t="s">
+      <c r="C43" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K43" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K44" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="L23" s="21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" s="21" t="s">
+      <c r="E45" s="10">
+        <v>1</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I45" s="11"/>
+    </row>
+    <row r="46" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="K24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="K25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K26" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="K47" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="12">
-        <v>1</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K30" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="10">
-        <v>1</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="K33" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K34" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="L34" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="K35" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K36" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K37" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="8">
-        <v>1</v>
-      </c>
-      <c r="L38" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K39" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K41" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="H43" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="I43" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="J43" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="K43" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="L43" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="20">
-        <v>1</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="L44" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="L46" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="K47" s="19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="K48" s="19" t="b">
+      <c r="K48" s="4" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M41" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:M30" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B958AC-AE9C-6646-926B-247F9F6B40B5}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071DF56E-A035-474F-A911-CCD631F267C6}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071DF56E-A035-474F-A911-CCD631F267C6}">
-  <dimension ref="A1:K6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1906,19 +1884,19 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>50</v>
@@ -1926,7 +1904,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
@@ -1946,7 +1924,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -1966,10 +1944,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>51</v>
@@ -1978,56 +1956,76 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" t="s">
         <v>97</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>98</v>
-      </c>
-      <c r="J4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F6" t="s">
         <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J6" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2036,12 +2034,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552128E9-1EC3-674C-BB17-36DDC2F16F66}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2058,10 +2056,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
@@ -2084,13 +2082,13 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>40</v>
@@ -2113,7 +2111,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>41</v>
@@ -2151,11 +2149,82 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B958AC-AE9C-6646-926B-247F9F6B40B5}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E48FB8-ACCC-E246-A2FC-0A7B1DE9E4F7}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B22190B-E02F-B743-AD1F-C6A98334425D}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2176,7 +2245,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: updated cohort model from 'table' to 'dataset'
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CohortsLocal.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CohortsLocal.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA0F9DF-3BEE-744E-90F3-5C9271F5A8B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF4CDDE-7266-B742-A070-D415FC792994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
     <sheet name="MyCollections" sheetId="15" r:id="rId2"/>
-    <sheet name="MyTables" sheetId="3" r:id="rId3"/>
+    <sheet name="MyDatasets" sheetId="3" r:id="rId3"/>
     <sheet name="MyVariables" sheetId="4" r:id="rId4"/>
     <sheet name="MyVariableHarmonisations" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -41,14 +41,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>table</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>Variables</t>
   </si>
   <si>
-    <t>Tables</t>
-  </si>
-  <si>
     <t>repeatsVariable</t>
   </si>
   <si>
@@ -118,15 +112,6 @@
     <t>syntax</t>
   </si>
   <si>
-    <t>TableHarmonisations</t>
-  </si>
-  <si>
-    <t>sourceTable</t>
-  </si>
-  <si>
-    <t>targetTable</t>
-  </si>
-  <si>
     <t>referencesVariable</t>
   </si>
   <si>
@@ -151,9 +136,6 @@
     <t>repeatsTable</t>
   </si>
   <si>
-    <t>MyTables</t>
-  </si>
-  <si>
     <t>refSchema</t>
   </si>
   <si>
@@ -175,9 +157,6 @@
     <t>MyVariableHarmonisations</t>
   </si>
   <si>
-    <t>MyTableHarmonisations</t>
-  </si>
-  <si>
     <t>MyCollection</t>
   </si>
   <si>
@@ -200,6 +179,30 @@
   </si>
   <si>
     <t>CodeLists</t>
+  </si>
+  <si>
+    <t>Datasets</t>
+  </si>
+  <si>
+    <t>MyDatasets</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>targetDataset</t>
+  </si>
+  <si>
+    <t>sourceDataset</t>
+  </si>
+  <si>
+    <t>MyDatasetHarmonisations</t>
+  </si>
+  <si>
+    <t>DatasetHarmonisations</t>
+  </si>
+  <si>
+    <t>acronym</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,112 +602,112 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -718,19 +721,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +746,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,35 +759,35 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -798,87 +801,87 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -892,7 +895,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,28 +910,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>